<commit_message>
Commit ke 12 dari jimmy
</commit_message>
<xml_diff>
--- a/Burndownchart.xlsx
+++ b/Burndownchart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Scrummaster" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="1.2" sheetId="3" r:id="rId3"/>
     <sheet name="1.3" sheetId="4" r:id="rId4"/>
     <sheet name="1.4" sheetId="5" r:id="rId5"/>
+    <sheet name="2.1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="33">
   <si>
     <t>SPRINT 1 :</t>
   </si>
@@ -93,6 +94,30 @@
   </si>
   <si>
     <t>Burnt Down Chart Sprint 1 - Hari Ketiga</t>
+  </si>
+  <si>
+    <t>Jumat</t>
+  </si>
+  <si>
+    <t>Sabtu</t>
+  </si>
+  <si>
+    <t>Minggu</t>
+  </si>
+  <si>
+    <t>Question Tag</t>
+  </si>
+  <si>
+    <t>Conditional Sentence</t>
+  </si>
+  <si>
+    <t>Many &amp; Much</t>
+  </si>
+  <si>
+    <t>Preposition</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -472,6 +497,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -492,21 +532,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -546,10 +571,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12357174103237098"/>
+          <c:x val="0.12357174103237101"/>
           <c:y val="0.1901738845144357"/>
           <c:w val="0.82153937007874001"/>
-          <c:h val="0.6548221055701372"/>
+          <c:h val="0.65482210557013731"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -611,24 +636,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="93448064"/>
-        <c:axId val="93449600"/>
+        <c:axId val="37795328"/>
+        <c:axId val="37796864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93448064"/>
+        <c:axId val="37795328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93449600"/>
+        <c:crossAx val="37796864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93449600"/>
+        <c:axId val="37796864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -636,7 +661,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93448064"/>
+        <c:crossAx val="37795328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -645,7 +670,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -734,25 +759,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="95776128"/>
-        <c:axId val="95810688"/>
+        <c:axId val="37981184"/>
+        <c:axId val="58721024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95776128"/>
+        <c:axId val="37981184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95810688"/>
+        <c:crossAx val="58721024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95810688"/>
+        <c:axId val="58721024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -760,7 +785,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95776128"/>
+        <c:crossAx val="37981184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -769,7 +794,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -863,24 +888,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="93455872"/>
-        <c:axId val="93509888"/>
+        <c:axId val="58761600"/>
+        <c:axId val="58763136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93455872"/>
+        <c:axId val="58761600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93509888"/>
+        <c:crossAx val="58763136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93509888"/>
+        <c:axId val="58763136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -888,7 +913,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93455872"/>
+        <c:crossAx val="58761600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -897,7 +922,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -933,10 +958,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10968285214348207"/>
-          <c:y val="0.19491907261592301"/>
-          <c:w val="0.70044203849518805"/>
-          <c:h val="0.67099883347914846"/>
+          <c:x val="0.10968285214348208"/>
+          <c:y val="0.19491907261592303"/>
+          <c:w val="0.70044203849518816"/>
+          <c:h val="0.6709988334791489"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1001,24 +1026,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62353792"/>
-        <c:axId val="62355328"/>
+        <c:axId val="58816000"/>
+        <c:axId val="58817536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="62353792"/>
+        <c:axId val="58816000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62355328"/>
+        <c:crossAx val="58817536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62355328"/>
+        <c:axId val="58817536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1026,7 +1051,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62353792"/>
+        <c:crossAx val="58816000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1035,7 +1060,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1549,7 +1574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
@@ -1559,15 +1584,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" t="s">
@@ -1576,11 +1601,11 @@
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1"/>
     <row r="6" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="25"/>
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1595,11 +1620,11 @@
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="22"/>
       <c r="E7" s="3">
         <v>10</v>
       </c>
@@ -1608,11 +1633,11 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="13"/>
-      <c r="D8" s="22"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="4">
         <v>40</v>
       </c>
@@ -1621,11 +1646,11 @@
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="13"/>
-      <c r="D9" s="22"/>
+      <c r="D9" s="15"/>
       <c r="E9" s="4">
         <v>40</v>
       </c>
@@ -1634,11 +1659,11 @@
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="13"/>
-      <c r="D10" s="22"/>
+      <c r="D10" s="15"/>
       <c r="E10" s="4">
         <v>40</v>
       </c>
@@ -1647,11 +1672,11 @@
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="5">
         <v>40</v>
       </c>
@@ -1709,15 +1734,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" t="s">
@@ -1726,11 +1751,11 @@
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1"/>
     <row r="6" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="25"/>
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1745,11 +1770,11 @@
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="22"/>
       <c r="E7" s="3">
         <v>10</v>
       </c>
@@ -1760,11 +1785,11 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="13"/>
-      <c r="D8" s="22"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="4">
         <v>40</v>
       </c>
@@ -1775,11 +1800,11 @@
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="13"/>
-      <c r="D9" s="22"/>
+      <c r="D9" s="15"/>
       <c r="E9" s="4">
         <v>40</v>
       </c>
@@ -1790,11 +1815,11 @@
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="13"/>
-      <c r="D10" s="22"/>
+      <c r="D10" s="15"/>
       <c r="E10" s="4">
         <v>40</v>
       </c>
@@ -1805,11 +1830,11 @@
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="5">
         <v>40</v>
       </c>
@@ -1866,15 +1891,15 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="2:8">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" t="s">
@@ -1883,11 +1908,11 @@
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1"/>
     <row r="6" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="25"/>
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1902,11 +1927,11 @@
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="22"/>
       <c r="E7" s="3">
         <v>10</v>
       </c>
@@ -1919,11 +1944,11 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="13"/>
-      <c r="D8" s="22"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="4">
         <v>40</v>
       </c>
@@ -1936,11 +1961,11 @@
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="13"/>
-      <c r="D9" s="22"/>
+      <c r="D9" s="15"/>
       <c r="E9" s="4">
         <v>40</v>
       </c>
@@ -1953,11 +1978,11 @@
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="13"/>
-      <c r="D10" s="22"/>
+      <c r="D10" s="15"/>
       <c r="E10" s="4">
         <v>40</v>
       </c>
@@ -1970,11 +1995,11 @@
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="5">
         <v>40</v>
       </c>
@@ -2026,22 +2051,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="2:8">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" t="s">
@@ -2050,11 +2075,11 @@
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1"/>
     <row r="6" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="25"/>
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
@@ -2069,11 +2094,11 @@
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="22"/>
       <c r="E7" s="3">
         <v>10</v>
       </c>
@@ -2088,11 +2113,11 @@
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="13"/>
-      <c r="D8" s="22"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="4">
         <v>40</v>
       </c>
@@ -2107,11 +2132,11 @@
       </c>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="13"/>
-      <c r="D9" s="22"/>
+      <c r="D9" s="15"/>
       <c r="E9" s="4">
         <v>40</v>
       </c>
@@ -2126,11 +2151,11 @@
       </c>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="13"/>
-      <c r="D10" s="22"/>
+      <c r="D10" s="15"/>
       <c r="E10" s="4">
         <v>40</v>
       </c>
@@ -2145,11 +2170,11 @@
       </c>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="5">
         <v>40</v>
       </c>
@@ -2186,15 +2211,151 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="2:7">
+      <c r="B2" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="15.75" thickBot="1"/>
+    <row r="6" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B6" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="3">
+        <v>100</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="4">
+        <v>100</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="15.75" thickBot="1">
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="6">
+        <f>SUM(E7:E10)</f>
+        <v>200</v>
+      </c>
+      <c r="F11" s="11">
+        <f>SUM(F7:F10)</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="11">
+        <f>SUM(G7:G10)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit ke tujuh belas dari jimmy
</commit_message>
<xml_diff>
--- a/Burndownchart.xlsx
+++ b/Burndownchart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Scrummaster" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,15 @@
     <sheet name="1.3" sheetId="4" r:id="rId4"/>
     <sheet name="1.4" sheetId="5" r:id="rId5"/>
     <sheet name="2.1" sheetId="6" r:id="rId6"/>
+    <sheet name="2.2" sheetId="8" r:id="rId7"/>
+    <sheet name="2.3" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="39">
   <si>
     <t>SPRINT 1 :</t>
   </si>
@@ -117,7 +119,25 @@
     <t>Preposition</t>
   </si>
   <si>
-    <t>-</t>
+    <t>Degree of Comparison</t>
+  </si>
+  <si>
+    <t>Passive Voice Part I</t>
+  </si>
+  <si>
+    <t>Passive Voice Part II</t>
+  </si>
+  <si>
+    <t>Passive Voice Part III</t>
+  </si>
+  <si>
+    <t>Passive Voice Part IV</t>
+  </si>
+  <si>
+    <t>Sythesis</t>
+  </si>
+  <si>
+    <t>Modal &amp; Auxiliaries</t>
   </si>
 </sst>
 </file>
@@ -148,7 +168,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -454,11 +474,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -490,6 +534,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -533,6 +586,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,7 +625,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout>
@@ -571,10 +632,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12357174103237101"/>
+          <c:x val="0.12357174103237106"/>
           <c:y val="0.1901738845144357"/>
           <c:w val="0.82153937007874001"/>
-          <c:h val="0.65482210557013731"/>
+          <c:h val="0.65482210557013754"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -636,24 +697,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="37795328"/>
-        <c:axId val="37796864"/>
+        <c:axId val="76212096"/>
+        <c:axId val="76213632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="37795328"/>
+        <c:axId val="76212096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37796864"/>
+        <c:crossAx val="76213632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37796864"/>
+        <c:axId val="76213632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,7 +722,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37795328"/>
+        <c:crossAx val="76212096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -670,7 +731,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -696,7 +757,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -759,25 +819,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="37981184"/>
-        <c:axId val="58721024"/>
+        <c:axId val="35122560"/>
+        <c:axId val="35402880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="37981184"/>
+        <c:axId val="35122560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58721024"/>
+        <c:crossAx val="35402880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58721024"/>
+        <c:axId val="35402880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -785,7 +845,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37981184"/>
+        <c:crossAx val="35122560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -794,7 +854,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -888,24 +948,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="58761600"/>
-        <c:axId val="58763136"/>
+        <c:axId val="35447552"/>
+        <c:axId val="35449088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="58761600"/>
+        <c:axId val="35447552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58763136"/>
+        <c:crossAx val="35449088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58763136"/>
+        <c:axId val="35449088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -913,7 +973,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58761600"/>
+        <c:crossAx val="35447552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -922,7 +982,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -958,10 +1018,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10968285214348208"/>
-          <c:y val="0.19491907261592303"/>
-          <c:w val="0.70044203849518816"/>
-          <c:h val="0.6709988334791489"/>
+          <c:x val="0.10968285214348211"/>
+          <c:y val="0.19491907261592309"/>
+          <c:w val="0.7004420384951886"/>
+          <c:h val="0.67099883347914957"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1026,24 +1086,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="58816000"/>
-        <c:axId val="58817536"/>
+        <c:axId val="58443648"/>
+        <c:axId val="58445184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="58816000"/>
+        <c:axId val="58443648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58817536"/>
+        <c:crossAx val="58445184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58817536"/>
+        <c:axId val="58445184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1051,7 +1111,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58816000"/>
+        <c:crossAx val="58443648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1060,7 +1120,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1503,21 +1563,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="13"/>
+      <c r="D4" s="16"/>
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1526,10 +1586,10 @@
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="13"/>
+      <c r="D5" s="16"/>
       <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1538,10 +1598,10 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="13"/>
+      <c r="D6" s="16"/>
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1550,10 +1610,10 @@
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="13"/>
+      <c r="D7" s="16"/>
       <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1584,15 +1644,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" t="s">
@@ -1601,11 +1661,11 @@
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1"/>
     <row r="6" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="25"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1620,11 +1680,11 @@
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="3">
         <v>10</v>
       </c>
@@ -1633,11 +1693,11 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="4">
         <v>40</v>
       </c>
@@ -1646,11 +1706,11 @@
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="4">
         <v>40</v>
       </c>
@@ -1659,11 +1719,11 @@
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="4">
         <v>40</v>
       </c>
@@ -1672,11 +1732,11 @@
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
       <c r="E11" s="5">
         <v>40</v>
       </c>
@@ -1725,7 +1785,7 @@
   <dimension ref="B2:H12"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H11" sqref="G7:H11"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1734,15 +1794,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" t="s">
@@ -1751,11 +1811,11 @@
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1"/>
     <row r="6" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="25"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1770,11 +1830,11 @@
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="3">
         <v>10</v>
       </c>
@@ -1785,11 +1845,11 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="4">
         <v>40</v>
       </c>
@@ -1800,11 +1860,11 @@
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="4">
         <v>40</v>
       </c>
@@ -1815,11 +1875,11 @@
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="4">
         <v>40</v>
       </c>
@@ -1830,11 +1890,11 @@
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
       <c r="E11" s="5">
         <v>40</v>
       </c>
@@ -1891,15 +1951,15 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="2:8">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" t="s">
@@ -1908,11 +1968,11 @@
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1"/>
     <row r="6" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="25"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1927,11 +1987,11 @@
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="3">
         <v>10</v>
       </c>
@@ -1944,11 +2004,11 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="4">
         <v>40</v>
       </c>
@@ -1961,11 +2021,11 @@
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="4">
         <v>40</v>
       </c>
@@ -1978,11 +2038,11 @@
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="4">
         <v>40</v>
       </c>
@@ -1995,11 +2055,11 @@
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
       <c r="E11" s="5">
         <v>40</v>
       </c>
@@ -2051,22 +2111,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="2:8">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" t="s">
@@ -2075,11 +2135,11 @@
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1"/>
     <row r="6" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="25"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
@@ -2094,11 +2154,11 @@
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="3">
         <v>10</v>
       </c>
@@ -2113,11 +2173,11 @@
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="4">
         <v>40</v>
       </c>
@@ -2132,11 +2192,11 @@
       </c>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="4">
         <v>40</v>
       </c>
@@ -2151,11 +2211,11 @@
       </c>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="4">
         <v>40</v>
       </c>
@@ -2170,11 +2230,11 @@
       </c>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
       <c r="E11" s="5">
         <v>40</v>
       </c>
@@ -2211,13 +2271,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2226,23 +2286,27 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:G11"/>
+  <dimension ref="B2:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="E15:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:7">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" t="s">
@@ -2251,11 +2315,11 @@
     </row>
     <row r="5" spans="2:7" ht="15.75" thickBot="1"/>
     <row r="6" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="25"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
       <c r="E6" s="2" t="s">
         <v>25</v>
       </c>
@@ -2267,95 +2331,651 @@
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="3">
-        <v>100</v>
-      </c>
-      <c r="F7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="4">
+        <v>35</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="4">
+        <v>30</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="4">
+        <v>30</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="4">
+        <v>30</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="4">
+        <v>30</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="4">
+        <v>30</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="30"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="4">
+        <v>20</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="4">
+        <v>35</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7">
-      <c r="B8" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="4">
-        <v>100</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7">
-      <c r="B10" s="14" t="s">
+      <c r="C16" s="30"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="4">
+        <v>25</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="15.75" thickBot="1">
-      <c r="D11" t="s">
+      <c r="C17" s="16"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="4">
+        <v>25</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="2:7" ht="15.75" thickBot="1">
+      <c r="D18" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="6">
-        <f>SUM(E7:E10)</f>
-        <v>200</v>
-      </c>
-      <c r="F11" s="11">
-        <f>SUM(F7:F10)</f>
+      <c r="E18" s="6">
+        <f>SUM(E7:E17)</f>
+        <v>320</v>
+      </c>
+      <c r="F18" s="11">
+        <f>SUM(F7:F17)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="11">
-        <f>SUM(G7:G10)</f>
+      <c r="G18" s="11">
+        <f>SUM(G7:G17)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B14:D14"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:G18"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7">
+      <c r="B2" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="15.75" thickBot="1"/>
+    <row r="6" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B6" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="3">
+        <v>30</v>
+      </c>
+      <c r="F7" s="8">
+        <v>10</v>
+      </c>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="4">
+        <v>35</v>
+      </c>
+      <c r="F8" s="8">
+        <v>20</v>
+      </c>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="4">
+        <v>30</v>
+      </c>
+      <c r="F9" s="8">
+        <v>30</v>
+      </c>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="4">
+        <v>30</v>
+      </c>
+      <c r="F10" s="8">
+        <v>30</v>
+      </c>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="4">
+        <v>30</v>
+      </c>
+      <c r="F11" s="8">
+        <v>30</v>
+      </c>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="4">
+        <v>30</v>
+      </c>
+      <c r="F12" s="8">
+        <v>30</v>
+      </c>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="4">
+        <v>30</v>
+      </c>
+      <c r="F13" s="8">
+        <v>20</v>
+      </c>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="30"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="4">
+        <v>20</v>
+      </c>
+      <c r="F14" s="8">
+        <v>20</v>
+      </c>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="4">
+        <v>35</v>
+      </c>
+      <c r="F15" s="8">
+        <v>35</v>
+      </c>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="4">
+        <v>25</v>
+      </c>
+      <c r="F16" s="8">
+        <v>25</v>
+      </c>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="4">
+        <v>25</v>
+      </c>
+      <c r="F17" s="8">
+        <v>25</v>
+      </c>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="2:7" ht="15.75" thickBot="1">
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="6">
+        <f>SUM(E7:E17)</f>
+        <v>320</v>
+      </c>
+      <c r="F18" s="11">
+        <f>SUM(F7:F17)</f>
+        <v>275</v>
+      </c>
+      <c r="G18" s="11">
+        <f>SUM(G7:G17)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B16:D16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:G18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7">
+      <c r="B2" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="15.75" thickBot="1"/>
+    <row r="6" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B6" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="3">
+        <v>30</v>
+      </c>
+      <c r="F7" s="8">
+        <v>10</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="4">
+        <v>35</v>
+      </c>
+      <c r="F8" s="8">
+        <v>20</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="4">
+        <v>30</v>
+      </c>
+      <c r="F9" s="8">
+        <v>30</v>
+      </c>
+      <c r="G9" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="4">
+        <v>30</v>
+      </c>
+      <c r="F10" s="8">
+        <v>30</v>
+      </c>
+      <c r="G10" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="4">
+        <v>30</v>
+      </c>
+      <c r="F11" s="8">
+        <v>30</v>
+      </c>
+      <c r="G11" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="4">
+        <v>30</v>
+      </c>
+      <c r="F12" s="8">
+        <v>30</v>
+      </c>
+      <c r="G12" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="4">
+        <v>30</v>
+      </c>
+      <c r="F13" s="8">
+        <v>20</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="30"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="4">
+        <v>20</v>
+      </c>
+      <c r="F14" s="8">
+        <v>20</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="4">
+        <v>35</v>
+      </c>
+      <c r="F15" s="8">
+        <v>35</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="4">
+        <v>25</v>
+      </c>
+      <c r="F16" s="8">
+        <v>25</v>
+      </c>
+      <c r="G16" s="8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="4">
+        <v>25</v>
+      </c>
+      <c r="F17" s="8">
+        <v>25</v>
+      </c>
+      <c r="G17" s="8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="15.75" thickBot="1">
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="6">
+        <f>SUM(E7:E17)</f>
+        <v>320</v>
+      </c>
+      <c r="F18" s="11">
+        <f>SUM(F7:F17)</f>
+        <v>275</v>
+      </c>
+      <c r="G18" s="11">
+        <f>SUM(G7:G17)</f>
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B16:D16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>